<commit_message>
fixed size for pictures
</commit_message>
<xml_diff>
--- a/blocksList.xlsx
+++ b/blocksList.xlsx
@@ -377,8 +377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A37" sqref="A20:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
add sentences under pictures
</commit_message>
<xml_diff>
--- a/blocksList.xlsx
+++ b/blocksList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
   <si>
     <t>jitter1</t>
   </si>
@@ -35,12 +35,6 @@
     <t>stimulus</t>
   </si>
   <si>
-    <t>VAS2</t>
-  </si>
-  <si>
-    <t>VAS8</t>
-  </si>
-  <si>
     <t>pictures\bad1.png</t>
   </si>
   <si>
@@ -51,12 +45,6 @@
   </si>
   <si>
     <t>pictures\neutral2.png</t>
-  </si>
-  <si>
-    <t>pictures\bad3.png</t>
-  </si>
-  <si>
-    <t>pictures\neutral3.png</t>
   </si>
 </sst>
 </file>
@@ -375,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A37" sqref="A20:XFD37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -403,7 +391,7 @@
         <v>1.653</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>0.84699999999999998</v>
@@ -414,7 +402,7 @@
         <v>1.736</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>0.76400000000000001</v>
@@ -425,7 +413,7 @@
         <v>1.653</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>0.84699999999999998</v>
@@ -436,7 +424,7 @@
         <v>1.736</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>0.76400000000000001</v>
@@ -447,7 +435,7 @@
         <v>1.653</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>0.84699999999999998</v>
@@ -458,7 +446,7 @@
         <v>1.736</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>0.76400000000000001</v>
@@ -469,7 +457,7 @@
         <v>1.653</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>0.84699999999999998</v>
@@ -480,7 +468,7 @@
         <v>1.736</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>0.76400000000000001</v>
@@ -491,7 +479,7 @@
         <v>1.653</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>0.84699999999999998</v>
@@ -502,7 +490,7 @@
         <v>1.736</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C11">
         <v>0.76400000000000001</v>
@@ -513,7 +501,7 @@
         <v>1.653</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>0.84699999999999998</v>
@@ -524,7 +512,7 @@
         <v>1.736</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C13">
         <v>0.76400000000000001</v>
@@ -535,7 +523,7 @@
         <v>1.653</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>0.84699999999999998</v>
@@ -546,7 +534,7 @@
         <v>1.736</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C15">
         <v>0.76400000000000001</v>
@@ -557,7 +545,7 @@
         <v>1.653</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C16">
         <v>0.84699999999999998</v>
@@ -568,231 +556,38 @@
         <v>1.736</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C17">
         <v>0.76400000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>1.653</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18">
-        <v>0.84699999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>1.736</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19">
-        <v>0.76400000000000001</v>
-      </c>
+      <c r="A18" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>1.653</v>
-      </c>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20">
-        <v>0.84699999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>1.736</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21">
-        <v>0.76400000000000001</v>
-      </c>
+      <c r="A20" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>1.653</v>
-      </c>
-      <c r="B22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22">
-        <v>0.84699999999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>1.736</v>
-      </c>
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23">
-        <v>0.76400000000000001</v>
-      </c>
+      <c r="A22" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>1.653</v>
-      </c>
-      <c r="B24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24">
-        <v>0.84699999999999998</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>1.736</v>
-      </c>
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25">
-        <v>0.76400000000000001</v>
-      </c>
+      <c r="A24" s="1"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>1.653</v>
-      </c>
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26">
-        <v>0.84699999999999998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>1.736</v>
-      </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27">
-        <v>0.76400000000000001</v>
-      </c>
+      <c r="A26" s="1"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>1.653</v>
-      </c>
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28">
-        <v>0.84699999999999998</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>1.736</v>
-      </c>
-      <c r="B29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29">
-        <v>0.76400000000000001</v>
-      </c>
+      <c r="A28" s="1"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
-        <v>1.653</v>
-      </c>
-      <c r="B30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30">
-        <v>0.84699999999999998</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>1.736</v>
-      </c>
-      <c r="B31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31">
-        <v>0.76400000000000001</v>
-      </c>
+      <c r="A30" s="1"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
-        <v>1.653</v>
-      </c>
-      <c r="B32" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32">
-        <v>0.84699999999999998</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>1.736</v>
-      </c>
-      <c r="B33" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33">
-        <v>0.76400000000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>1.653</v>
-      </c>
-      <c r="B34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34">
-        <v>0.84699999999999998</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>1.736</v>
-      </c>
-      <c r="B35" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35">
-        <v>0.76400000000000001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
-        <v>1.653</v>
-      </c>
-      <c r="B36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36">
-        <v>0.84699999999999998</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>1.736</v>
-      </c>
-      <c r="B37" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37">
-        <v>0.76400000000000001</v>
-      </c>
+      <c r="A32" s="1"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changes after meeting in the MRI
Changes after meeting in the MRI:
remove half degrees
ask sooner in the calibration (after 5 seconds from target temp)
devide to 2 runs
always show fixation
remove sleep(2) and add another stimulus instead
</commit_message>
<xml_diff>
--- a/blocksList.xlsx
+++ b/blocksList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t>jitter1</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>pictures\neutral2.png</t>
+  </si>
+  <si>
+    <t>VAS2</t>
+  </si>
+  <si>
+    <t>VAS8</t>
   </si>
 </sst>
 </file>
@@ -365,8 +371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -457,7 +463,7 @@
         <v>1.653</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>0.84699999999999998</v>
@@ -468,7 +474,7 @@
         <v>1.736</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <v>0.76400000000000001</v>
@@ -479,7 +485,7 @@
         <v>1.653</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>0.84699999999999998</v>
@@ -490,7 +496,7 @@
         <v>1.736</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>0.76400000000000001</v>
@@ -501,7 +507,7 @@
         <v>1.653</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C12">
         <v>0.84699999999999998</v>
@@ -512,7 +518,7 @@
         <v>1.736</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C13">
         <v>0.76400000000000001</v>
@@ -523,7 +529,7 @@
         <v>1.653</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C14">
         <v>0.84699999999999998</v>
@@ -534,7 +540,7 @@
         <v>1.736</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C15">
         <v>0.76400000000000001</v>
@@ -545,7 +551,7 @@
         <v>1.653</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C16">
         <v>0.84699999999999998</v>
@@ -556,7 +562,7 @@
         <v>1.736</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C17">
         <v>0.76400000000000001</v>
@@ -591,5 +597,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>